<commit_message>
nuget pkgs vers. in MacOS_Ver_NugetPkgs.xlsx
</commit_message>
<xml_diff>
--- a/MacOS_Ver_NugetPkgs.xlsx
+++ b/MacOS_Ver_NugetPkgs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\eigil\projects\xamarinProjs\TimeDateCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{6217F1DC-5DEB-451A-A0D1-D94A5331542E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0373C6E-F53E-40F8-AB7C-C8254DC5E36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <r>
       <rPr>
@@ -163,6 +163,90 @@
         <rFont val="Arial"/>
       </rPr>
       <t>4.7.0.1351</t>
+    </r>
+  </si>
+  <si>
+    <t>macOS_Ver</t>
+  </si>
+  <si>
+    <t>Ver.__3.6.21.1._Uploaded_to_Mac-_App_Stpre_Connect</t>
+  </si>
+  <si>
+    <t>TimeDateCalculator.macOS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Xamarin.Essentials by Microsoft</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1.6.0-pre2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1.6.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Xamarin.Essentials: a kit of essential API's for your apps</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Xamarin.Forms by Microsoft</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Build native Uis for iOS, Android, UWP, macOS, Tizen and many more from a single, shared C# codebase</t>
+    </r>
+  </si>
+  <si>
+    <t>TimeDateCalculatorDLL</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>4.8.0.1560</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Build native UIs for iOS, Android, UWP, macOS, Tizen and many more from a single, shared C# codebase</t>
     </r>
   </si>
 </sst>
@@ -170,10 +254,37 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -310,6 +421,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,11 +739,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.42578125"/>
     <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
@@ -636,104 +753,216 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>